<commit_message>
updated ingredients list class
</commit_message>
<xml_diff>
--- a/Ingredients.xlsx
+++ b/Ingredients.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmman\git\Recipe_Scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7506A2FA-E4ED-46E4-853C-8F13D2A03BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CEA7FE-3C73-477B-A538-9451BE996FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LFV" sheetId="5" r:id="rId1"/>
     <sheet name="LCHF" sheetId="6" r:id="rId2"/>
     <sheet name="Allergies" sheetId="7" r:id="rId3"/>
+    <sheet name="Food_Category" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="286">
   <si>
     <t>LFV_FullVegan_Eliminate</t>
   </si>
@@ -751,6 +752,135 @@
   </si>
   <si>
     <t>Seafood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foodcategory </t>
+  </si>
+  <si>
+    <t>cuisinecategory</t>
+  </si>
+  <si>
+    <t>recipecategory</t>
+  </si>
+  <si>
+    <t>Vegan</t>
+  </si>
+  <si>
+    <t>Vegetarian</t>
+  </si>
+  <si>
+    <t>Jain</t>
+  </si>
+  <si>
+    <t>Eggitarian</t>
+  </si>
+  <si>
+    <t>Non-veg</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>South Indian</t>
+  </si>
+  <si>
+    <t>Rajasthani</t>
+  </si>
+  <si>
+    <t>Punjabi</t>
+  </si>
+  <si>
+    <t>Bengali</t>
+  </si>
+  <si>
+    <t>orissa</t>
+  </si>
+  <si>
+    <t>Gujarati</t>
+  </si>
+  <si>
+    <t>Maharashtrian</t>
+  </si>
+  <si>
+    <t>Andhra</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>Goan</t>
+  </si>
+  <si>
+    <t>Kashmiri</t>
+  </si>
+  <si>
+    <t>Himachali</t>
+  </si>
+  <si>
+    <t>Tamil nadu</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>Sindhi</t>
+  </si>
+  <si>
+    <t>Chhattisgarhi</t>
+  </si>
+  <si>
+    <t>Madhya pradesh</t>
+  </si>
+  <si>
+    <t>Assamese</t>
+  </si>
+  <si>
+    <t>Manipuri</t>
+  </si>
+  <si>
+    <t>Tripuri</t>
+  </si>
+  <si>
+    <t>Sikkimese</t>
+  </si>
+  <si>
+    <t>Mizo</t>
+  </si>
+  <si>
+    <t>Arunachali</t>
+  </si>
+  <si>
+    <t>uttarakhand</t>
+  </si>
+  <si>
+    <t>Haryanvi</t>
+  </si>
+  <si>
+    <t>Awadhi</t>
+  </si>
+  <si>
+    <t>Bihari</t>
+  </si>
+  <si>
+    <t>Uttar pradesh</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>North Indian</t>
+  </si>
+  <si>
+    <t>Breakfast</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>Snack</t>
+  </si>
+  <si>
+    <t>Dinner</t>
   </si>
 </sst>
 </file>
@@ -810,7 +940,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -848,23 +978,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1082,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50579E66-7B1E-40F2-8BB6-D390A5F734E5}">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2669,7 +2832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EBCD2A-CD24-4DB8-BDBA-7AC67F265BF4}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -2746,4 +2909,217 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D54DEA3-031C-4107-9637-F8D8F08D6C86}">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="10" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="12" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="12" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="12" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="12" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="12" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="12" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="12" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="12" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="12" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="12" t="s">
+        <v>281</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
sending pagination in a new file
</commit_message>
<xml_diff>
--- a/Ingredients.xlsx
+++ b/Ingredients.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmman\git\Recipe_Scraping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balbi\git\Recipe_Scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CEA7FE-3C73-477B-A538-9451BE996FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E82DEED-4AB8-410D-AA25-7E42657F7ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LFV" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="287">
   <si>
     <t>LFV_FullVegan_Eliminate</t>
   </si>
@@ -881,6 +881,9 @@
   </si>
   <si>
     <t>Dinner</t>
+  </si>
+  <si>
+    <t>Chana</t>
   </si>
 </sst>
 </file>
@@ -1010,7 +1013,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1023,11 +1026,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1246,7 +1248,7 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,7 +1278,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>286</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -2926,10 +2928,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>244</v>
       </c>
       <c r="C1" t="s">
@@ -2937,185 +2939,184 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="11" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="11" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="11" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="11" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="11" t="s">
         <v>281</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding pagination in lfv partial
</commit_message>
<xml_diff>
--- a/Ingredients.xlsx
+++ b/Ingredients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balbi\git\Recipe_Scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E82DEED-4AB8-410D-AA25-7E42657F7ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A1FB26-6972-4FA4-B944-941491F56CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -883,7 +883,7 @@
     <t>Dinner</t>
   </si>
   <si>
-    <t>Chana</t>
+    <t>chana</t>
   </si>
 </sst>
 </file>
@@ -1248,7 +1248,7 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
LFV working till page 20
</commit_message>
<xml_diff>
--- a/Ingredients.xlsx
+++ b/Ingredients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balbi\git\Recipe_Scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A1FB26-6972-4FA4-B944-941491F56CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EF2D9F-F6C1-4107-8DE0-12CA31E6382C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="1800" windowWidth="21600" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LFV" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="286">
   <si>
     <t>LFV_FullVegan_Eliminate</t>
   </si>
@@ -881,9 +881,6 @@
   </si>
   <si>
     <t>Dinner</t>
-  </si>
-  <si>
-    <t>chana</t>
   </si>
 </sst>
 </file>
@@ -1278,7 +1275,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>286</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>

</xml_diff>